<commit_message>
Neue Arbeitszeiten Rabe: 30-11-20
</commit_message>
<xml_diff>
--- a/ArbeitszeitRabe.xlsx
+++ b/ArbeitszeitRabe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45492bff350aaf01/Desktop/Dokumente/Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_AD4DB114E441178AC67DF4BE5E11D192683EDF1A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE57DAC7-4A08-497F-9B4B-C3426FD39489}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_AD4DB114E441178AC67DF4BE5E11D192683EDF1A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{46379623-6880-4CBC-89C2-2076E5301E24}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Datum</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>12 Uhr</t>
+  </si>
+  <si>
+    <t>Fertigstellung Basis Login System</t>
+  </si>
+  <si>
+    <t>8:00 Uhr</t>
+  </si>
+  <si>
+    <t>12:30 Uhr</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>13:00 Uhr</t>
+  </si>
+  <si>
+    <t>14:00 Uhr</t>
   </si>
 </sst>
 </file>
@@ -394,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F6"/>
+  <dimension ref="B3:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,7 +427,7 @@
     <col min="3" max="3" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>44159</v>
       </c>
@@ -440,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>44162</v>
       </c>
@@ -457,7 +478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>44164</v>
       </c>
@@ -472,6 +493,46 @@
       </c>
       <c r="F6">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>44165</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>44165</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Neue Arbeitszeit Florian Rabe
</commit_message>
<xml_diff>
--- a/ArbeitszeitRabe.xlsx
+++ b/ArbeitszeitRabe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45492bff350aaf01/Desktop/Dokumente/Dokumente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45492bff350aaf01/Desktop/web-projekte/BachelorProjekt/Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_AD4DB114E441178AC67DF4BE5E11D192683EDF1A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{46379623-6880-4CBC-89C2-2076E5301E24}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_AD4DB114E441178AC67DF4BE5E11D192683EDF1A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5C902627-2A06-479D-AD58-8785D2624FEE}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22140" yWindow="15" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>14:00 Uhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting + Webseite bauen (Slider + weiterer Div Bereich) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:00 Uhr </t>
+  </si>
+  <si>
+    <t>17:00 Uhr</t>
   </si>
 </sst>
 </file>
@@ -131,10 +140,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -415,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:H8"/>
+  <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,6 +545,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>44172</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>